<commit_message>
committing framework changes and keyword based
</commit_message>
<xml_diff>
--- a/TestData/RegisterCompany.xlsx
+++ b/TestData/RegisterCompany.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16485" windowHeight="3585"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16305" windowHeight="1680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A4:F13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t xml:space="preserve">Your Name </t>
   </si>
@@ -112,9 +112,6 @@
     <t>amet@sedt.edu</t>
   </si>
   <si>
-    <t>temp.clidiem.com</t>
-  </si>
-  <si>
     <t>amron@seiwr.co</t>
   </si>
   <si>
@@ -200,13 +197,43 @@
   </si>
   <si>
     <t>11-1234576</t>
+  </si>
+  <si>
+    <t>temp.clidiem1.com</t>
+  </si>
+  <si>
+    <t>temp.clidiem2.com</t>
+  </si>
+  <si>
+    <t>temp.clidiem3.com</t>
+  </si>
+  <si>
+    <t>temp.clidiem4.com</t>
+  </si>
+  <si>
+    <t>temp.clidiem5.com</t>
+  </si>
+  <si>
+    <t>temp.clidiem6.com</t>
+  </si>
+  <si>
+    <t>temp.clidiem7.com</t>
+  </si>
+  <si>
+    <t>temp.clidiem8.com</t>
+  </si>
+  <si>
+    <t>temp.clidiem9.com</t>
+  </si>
+  <si>
+    <t>temp.clidiem10.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,7 +396,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -404,7 +430,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -580,14 +605,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -599,7 +624,7 @@
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -607,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -628,27 +653,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E2">
-        <v>1992342387</v>
+        <v>1992342396</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>29</v>
@@ -657,7 +682,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -665,19 +690,19 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3">
         <v>1992342388</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>29</v>
@@ -686,7 +711,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -694,7 +719,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>30</v>
@@ -703,10 +728,10 @@
         <v>1992342389</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>29</v>
@@ -715,7 +740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -723,19 +748,19 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5">
         <v>1992342390</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>29</v>
@@ -744,7 +769,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -752,19 +777,19 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6">
         <v>1992342391</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>29</v>
@@ -773,7 +798,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -781,19 +806,19 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7">
         <v>1992342392</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>29</v>
@@ -802,7 +827,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -810,19 +835,19 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8">
         <v>1992342393</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>29</v>
@@ -831,7 +856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -839,19 +864,19 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9">
         <v>1992342394</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>29</v>
@@ -860,7 +885,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -868,19 +893,19 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10">
         <v>1992342395</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>29</v>
@@ -889,27 +914,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>1992342387</v>
+      </c>
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11">
-        <v>1992342396</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="G11" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>29</v>
@@ -920,9 +945,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="H2" r:id="rId2"/>
-    <hyperlink ref="I2" r:id="rId3"/>
+    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="H11" r:id="rId2"/>
+    <hyperlink ref="I11" r:id="rId3"/>
     <hyperlink ref="H3" r:id="rId4"/>
     <hyperlink ref="H4" r:id="rId5"/>
     <hyperlink ref="H5" r:id="rId6"/>
@@ -931,7 +956,7 @@
     <hyperlink ref="H8" r:id="rId9"/>
     <hyperlink ref="H9" r:id="rId10"/>
     <hyperlink ref="H10" r:id="rId11"/>
-    <hyperlink ref="H11" r:id="rId12"/>
+    <hyperlink ref="H2" r:id="rId12"/>
     <hyperlink ref="I3" r:id="rId13"/>
     <hyperlink ref="I4" r:id="rId14"/>
     <hyperlink ref="I5" r:id="rId15"/>
@@ -940,7 +965,7 @@
     <hyperlink ref="I8" r:id="rId18"/>
     <hyperlink ref="I9" r:id="rId19"/>
     <hyperlink ref="I10" r:id="rId20"/>
-    <hyperlink ref="I11" r:id="rId21"/>
+    <hyperlink ref="I2" r:id="rId21"/>
     <hyperlink ref="D4" r:id="rId22"/>
     <hyperlink ref="D5" r:id="rId23"/>
     <hyperlink ref="D6" r:id="rId24"/>
@@ -948,7 +973,7 @@
     <hyperlink ref="D8" r:id="rId26"/>
     <hyperlink ref="D9" r:id="rId27"/>
     <hyperlink ref="D10" r:id="rId28"/>
-    <hyperlink ref="D11" r:id="rId29"/>
+    <hyperlink ref="D2" r:id="rId29"/>
     <hyperlink ref="D3" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -956,24 +981,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>